<commit_message>
Login Google rebuild in React Produce JSON on demand Notify Service & Invitation user
</commit_message>
<xml_diff>
--- a/question Togh.xlsx
+++ b/question Togh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\togh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB21CE88-0B44-4CED-9C9B-72E91E1E57F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B63E83-81ED-4845-BCDB-E0AB2249D556}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5970" yWindow="435" windowWidth="15825" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="1875" windowWidth="21690" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -393,15 +393,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,16 +694,16 @@
     <col min="4" max="4" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="321" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -794,14 +794,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -826,11 +826,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -869,11 +869,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -891,106 +891,106 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="39" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="39" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="43" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="43" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="47" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-    </row>
-    <row r="53" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+    </row>
+    <row r="53" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-    </row>
-    <row r="57" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="57" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-    </row>
-    <row r="61" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="61" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="4" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>